<commit_message>
added graph to population page; resize works
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-40" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="110">
   <si>
     <t>Page or Event</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>array of boolean</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>interacts with the freezer</t>
+  </si>
+  <si>
+    <t>var name</t>
   </si>
 </sst>
 </file>
@@ -804,19 +813,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -824,1036 +833,1124 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" t="s">
         <v>52</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1"/>
+      <c r="D32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1"/>
+      <c r="D39" t="s">
         <v>54</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1"/>
+      <c r="D40" t="s">
         <v>55</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1"/>
+      <c r="D41" t="s">
         <v>56</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" t="s">
         <v>57</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" t="s">
         <v>58</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
         <v>59</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" t="s">
         <v>60</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
         <v>61</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
         <v>62</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1"/>
+      <c r="D51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>24</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1"/>
+      <c r="D55" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>24</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1"/>
+      <c r="D56" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>24</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1"/>
+      <c r="D57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1"/>
+      <c r="D58" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1"/>
+      <c r="D59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1"/>
+      <c r="D60" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1"/>
+      <c r="D61" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>24</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1"/>
+      <c r="D62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>24</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>24</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>76</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1"/>
+      <c r="D68" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:4">
       <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1"/>
+      <c r="D70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2"/>
+      <c r="D71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>80</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1"/>
+      <c r="D72" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:4">
       <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1"/>
+      <c r="D74" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1"/>
+      <c r="D75" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1"/>
+      <c r="D76" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1"/>
+      <c r="D77" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1"/>
+      <c r="D78" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1"/>
+      <c r="D79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1"/>
+      <c r="D80" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1"/>
+      <c r="D81" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1"/>
+      <c r="D82" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>79</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1"/>
+      <c r="D83" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1"/>
+      <c r="D84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>79</v>
       </c>
       <c r="B85" t="s">
         <v>37</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>79</v>
       </c>
       <c r="B86" t="s">
         <v>37</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>79</v>
       </c>
       <c r="B87" t="s">
         <v>4</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>79</v>
       </c>
       <c r="B88" t="s">
         <v>4</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>79</v>
       </c>
       <c r="B89" t="s">
         <v>4</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>79</v>
       </c>
       <c r="B90" t="s">
         <v>4</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>79</v>
       </c>
       <c r="B91" t="s">
         <v>4</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>79</v>
       </c>
       <c r="B92" t="s">
         <v>4</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>79</v>
       </c>
       <c r="B93" t="s">
         <v>4</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>79</v>
       </c>
       <c r="B94" t="s">
         <v>4</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>79</v>
       </c>
       <c r="B95" t="s">
         <v>4</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>107</v>
+      </c>
+      <c r="D97" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added information to notes folder on interface
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="2480" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="interface" sheetId="1" r:id="rId1"/>
+    <sheet name="freezer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="252">
   <si>
     <t>Page or Event</t>
   </si>
@@ -265,9 +265,6 @@
     <t>onLoad</t>
   </si>
   <si>
-    <t>genome</t>
-  </si>
-  <si>
     <t>when each function performed</t>
   </si>
   <si>
@@ -346,10 +343,439 @@
     <t>Analysis</t>
   </si>
   <si>
-    <t>interacts with the freezer</t>
-  </si>
-  <si>
     <t>var name</t>
+  </si>
+  <si>
+    <t>array of number</t>
+  </si>
+  <si>
+    <t>t0 = Average Fitness</t>
+  </si>
+  <si>
+    <t>t1=Average Gestation Time</t>
+  </si>
+  <si>
+    <t>t2 = Average Metabolic Rate</t>
+  </si>
+  <si>
+    <t>name in entryname.txt</t>
+  </si>
+  <si>
+    <t>t3 = Number of Organisms</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>get &amp; set</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>genome in genome.seq</t>
+  </si>
+  <si>
+    <t>*.avidaedworkspace</t>
+  </si>
+  <si>
+    <t>c0</t>
+  </si>
+  <si>
+    <t>root folder</t>
+  </si>
+  <si>
+    <t>subfolder</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>avida.cfg</t>
+  </si>
+  <si>
+    <t>environment.cfg</t>
+  </si>
+  <si>
+    <t>events.cfg</t>
+  </si>
+  <si>
+    <t>entryname.txt</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>same files as c0</t>
+  </si>
+  <si>
+    <t>etc</t>
+  </si>
+  <si>
+    <t>contents</t>
+  </si>
+  <si>
+    <t>WORLD_X 60</t>
+  </si>
+  <si>
+    <t>WORLD_Y 60</t>
+  </si>
+  <si>
+    <t>WORLD_GEOMETRY 1</t>
+  </si>
+  <si>
+    <t>COPY_MUT_PROB 0.02</t>
+  </si>
+  <si>
+    <t>DIVIDE_INS_PROB 0.0</t>
+  </si>
+  <si>
+    <t>DIVIDE_DEL_PROB 0.0</t>
+  </si>
+  <si>
+    <t>OFFSPRING_SIZE_RANGE 1.0</t>
+  </si>
+  <si>
+    <t>BIRTH_METHOD 0</t>
+  </si>
+  <si>
+    <t>RANDOM_SEED -1</t>
+  </si>
+  <si>
+    <t>#include instset.cfg</t>
+  </si>
+  <si>
+    <t>REACTION  NOT  not   process:value=1.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  NAND nand  process:value=1.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  AND  and   process:value=2.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  ORN  orn   process:value=2.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  OR   or    process:value=3.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  ANDN andn  process:value=3.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  NOR  nor   process:value=4.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  XOR  xor   process:value=4.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  EQU  equ   process:value=5.0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>@default</t>
+  </si>
+  <si>
+    <t>instset.cfg</t>
+  </si>
+  <si>
+    <t>INSTSET heads_default:hw_type=0</t>
+  </si>
+  <si>
+    <t># No-ops</t>
+  </si>
+  <si>
+    <t>INST nop-A         # a</t>
+  </si>
+  <si>
+    <t>INST nop-B         # b</t>
+  </si>
+  <si>
+    <t>INST nop-C         # c</t>
+  </si>
+  <si>
+    <t># Flow control operations</t>
+  </si>
+  <si>
+    <t>INST if-n-equ      # d</t>
+  </si>
+  <si>
+    <t>INST if-less       # e</t>
+  </si>
+  <si>
+    <t>INST if-label      # f</t>
+  </si>
+  <si>
+    <t>INST mov-head      # g</t>
+  </si>
+  <si>
+    <t>INST jmp-head      # h</t>
+  </si>
+  <si>
+    <t>INST get-head      # i</t>
+  </si>
+  <si>
+    <t>INST set-flow      # j</t>
+  </si>
+  <si>
+    <t># Single Argument Math</t>
+  </si>
+  <si>
+    <t>INST shift-r       # k</t>
+  </si>
+  <si>
+    <t>INST shift-l       # l</t>
+  </si>
+  <si>
+    <t>INST inc           # m</t>
+  </si>
+  <si>
+    <t>INST dec           # n</t>
+  </si>
+  <si>
+    <t>INST push          # o</t>
+  </si>
+  <si>
+    <t>INST pop           # p</t>
+  </si>
+  <si>
+    <t>INST swap-stk      # q</t>
+  </si>
+  <si>
+    <t>INST swap          # r</t>
+  </si>
+  <si>
+    <t># Double Argument Math</t>
+  </si>
+  <si>
+    <t>INST add           # s</t>
+  </si>
+  <si>
+    <t>INST sub           # t</t>
+  </si>
+  <si>
+    <t>INST nand          # u</t>
+  </si>
+  <si>
+    <t># Biological Operations</t>
+  </si>
+  <si>
+    <t>INST h-copy        # v</t>
+  </si>
+  <si>
+    <t>INST h-alloc       # w</t>
+  </si>
+  <si>
+    <t>INST h-divide      # x</t>
+  </si>
+  <si>
+    <t># I/O and Sensory</t>
+  </si>
+  <si>
+    <t>INST IO            # y</t>
+  </si>
+  <si>
+    <t>INST h-search      # z</t>
+  </si>
+  <si>
+    <t>g0</t>
+  </si>
+  <si>
+    <t>genome.seq</t>
+  </si>
+  <si>
+    <t>0,heads_default,wzcagcccccccccccccccccccccccccccccccccccczvfcaxgab</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>same files as g0</t>
+  </si>
+  <si>
+    <t>clade.ssg</t>
+  </si>
+  <si>
+    <t>#filetype systematics_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#format name cells </t>
+  </si>
+  <si>
+    <t># Structured Systematics Group Save</t>
+  </si>
+  <si>
+    <t># Tue May 19 16:50:39 2015</t>
+  </si>
+  <si>
+    <t>#  1: Clade Name</t>
+  </si>
+  <si>
+    <t>#  2: Occupied Cell IDs</t>
+  </si>
+  <si>
+    <t>@ancestor 0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. . . </t>
+  </si>
+  <si>
+    <t>#filetype genotype_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#format id src src_args parents num_units total_units length merit gest_time fitness gen_born update_born update_deactivated depth hw_type inst_set sequence cells gest_offset lineage </t>
+  </si>
+  <si>
+    <t># Structured Population Save</t>
+  </si>
+  <si>
+    <t>#  1: ID</t>
+  </si>
+  <si>
+    <t>#  2: Source</t>
+  </si>
+  <si>
+    <t>#  3: Source Args</t>
+  </si>
+  <si>
+    <t>#  4: Parent ID(s)</t>
+  </si>
+  <si>
+    <t>#  5: Number of currently living organisms</t>
+  </si>
+  <si>
+    <t>#  6: Total number of organisms that ever existed</t>
+  </si>
+  <si>
+    <t>#  7: Genome Length</t>
+  </si>
+  <si>
+    <t>#  8: Average Merit</t>
+  </si>
+  <si>
+    <t>#  9: Average Gestation Time</t>
+  </si>
+  <si>
+    <t># 10: Average Fitness</t>
+  </si>
+  <si>
+    <t># 11: Generation Born</t>
+  </si>
+  <si>
+    <t># 12: Update Born</t>
+  </si>
+  <si>
+    <t># 13: Update Deactivated</t>
+  </si>
+  <si>
+    <t># 14: Phylogenetic Depth</t>
+  </si>
+  <si>
+    <t># 15: Hardware Type ID</t>
+  </si>
+  <si>
+    <t># 16: Inst Set Name</t>
+  </si>
+  <si>
+    <t># 17: Genome Sequence</t>
+  </si>
+  <si>
+    <t># 18: Occupied Cell IDs</t>
+  </si>
+  <si>
+    <t># 19: Gestation (CPU) Cycle Offsets</t>
+  </si>
+  <si>
+    <t># 20: Lineage Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44735 div:int (none) 43210 1 3 50 46 130 0.353846 194 1001 -1 42 0 heads_default wzjagcufclcastcwvlvfciawxqcnrcuckczkmzrmszvfvvxglb 8 36 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">43930 div:int (none) 43681 3 7 50 47 136 0.345588 191 987 -1 44 0 heads_default wnjagcpfclcahtcoflflciawxqcnrcuccczqmtrmkzvfvvxglb 44,45,75 123,17,17 0,0,0 </t>
+  </si>
+  <si>
+    <t>detail.spop</t>
+  </si>
+  <si>
+    <t>w1</t>
+  </si>
+  <si>
+    <t>Im2-w30x30-1000-norewards</t>
+  </si>
+  <si>
+    <t>REACTION  NOT  not   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  NAND nand  process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  AND  and   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  ORN  orn   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  OR   or    process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  ANDN andn  process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  NOR  nor   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  XOR  xor   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>REACTION  EQU  equ   process:value=0:type=pow  requisite:max_count=1</t>
+  </si>
+  <si>
+    <t>u begin LoadPopulation detail.spop</t>
+  </si>
+  <si>
+    <t>u begin LoadStructuredSystematicsGroup  role=clade:filename=clade.ssg</t>
+  </si>
+  <si>
+    <t>same as file above</t>
+  </si>
+  <si>
+    <t>0:0.000000,1:0.000000,2:0.000000,3:0.000000,4:0.000000,5:0.000000,6:0.248677,7:0.248677,8:0.248677, etc</t>
+  </si>
+  <si>
+    <t>tr0=fitness</t>
+  </si>
+  <si>
+    <t>tr1=gestation time</t>
+  </si>
+  <si>
+    <t>tr3=number of organisms</t>
+  </si>
+  <si>
+    <t>tr2=metabolic rate</t>
+  </si>
+  <si>
+    <t>0:189.000000,1:189.000000,2:189.000000,3:189.000000,4:189.000000,5:189.000000,6:189.000000,7:189.000000,8:189.000000,etc</t>
+  </si>
+  <si>
+    <t>0:47.000000,1:47.000000,2:47.000000,3:47.000000,4:47.000000,5:47.000000,6:47.000000,7:47.000000,8:47.000000, etc</t>
+  </si>
+  <si>
+    <t>0:1.000000,1:1.000000,2:1.000000,3:1.000000,4:1.000000,5:1.000000,6:2.000000,7:2.000000,8:2.000000, etc</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>same files as w1</t>
+  </si>
+  <si>
+    <t>@ancestor</t>
   </si>
 </sst>
 </file>
@@ -403,7 +829,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -441,13 +867,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +915,17 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -484,6 +944,17 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -813,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -833,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1612,7 +2083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -1624,7 +2095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -1636,7 +2107,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -1648,11 +2119,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -1661,181 +2132,218 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>112</v>
+      </c>
+      <c r="E70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>80</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="2"/>
+      <c r="B71" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="1"/>
       <c r="D71" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="D72" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="C73" s="1"/>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>93</v>
+      </c>
+      <c r="E75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>91</v>
+      </c>
+      <c r="E76" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>92</v>
+      </c>
+      <c r="E77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>83</v>
+      </c>
+      <c r="E78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>84</v>
+      </c>
+      <c r="E79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>85</v>
+      </c>
+      <c r="E80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>87</v>
+      </c>
+      <c r="E82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>79</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>88</v>
+      </c>
+      <c r="E83" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>89</v>
+      </c>
+      <c r="E84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>79</v>
       </c>
-      <c r="B85" t="s">
-        <v>37</v>
-      </c>
+      <c r="B85" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" s="1"/>
       <c r="D85" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>90</v>
+      </c>
+      <c r="E85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -1843,21 +2351,27 @@
         <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>94</v>
+      </c>
+      <c r="E86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D87" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>95</v>
+      </c>
+      <c r="E87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>79</v>
       </c>
@@ -1865,10 +2379,13 @@
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>96</v>
+      </c>
+      <c r="E88" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>79</v>
       </c>
@@ -1876,10 +2393,13 @@
         <v>4</v>
       </c>
       <c r="D89" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>97</v>
+      </c>
+      <c r="E89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>79</v>
       </c>
@@ -1887,10 +2407,13 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="E90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>79</v>
       </c>
@@ -1898,10 +2421,13 @@
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>99</v>
+      </c>
+      <c r="E91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -1909,10 +2435,13 @@
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>100</v>
+      </c>
+      <c r="E92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>79</v>
       </c>
@@ -1920,10 +2449,13 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>101</v>
+      </c>
+      <c r="E93" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>79</v>
       </c>
@@ -1931,10 +2463,13 @@
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>102</v>
+      </c>
+      <c r="E94" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -1942,15 +2477,94 @@
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" t="s">
-        <v>107</v>
-      </c>
-      <c r="D97" t="s">
+        <v>103</v>
+      </c>
+      <c r="E95" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>104</v>
+      </c>
+      <c r="E96" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" t="s">
         <v>108</v>
+      </c>
+      <c r="D98" t="s">
+        <v>109</v>
+      </c>
+      <c r="E98" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" t="s">
+        <v>110</v>
+      </c>
+      <c r="E99" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" t="s">
+        <v>108</v>
+      </c>
+      <c r="D100" t="s">
+        <v>111</v>
+      </c>
+      <c r="E100" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" t="s">
+        <v>108</v>
+      </c>
+      <c r="D101" t="s">
+        <v>113</v>
+      </c>
+      <c r="E101" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1966,18 +2580,1697 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" t="s">
+        <v>187</v>
+      </c>
+      <c r="D64" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" t="s">
+        <v>189</v>
+      </c>
+      <c r="C66" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" t="s">
+        <v>226</v>
+      </c>
+      <c r="C69" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>118</v>
+      </c>
+      <c r="B71" t="s">
+        <v>226</v>
+      </c>
+      <c r="C71" t="s">
+        <v>191</v>
+      </c>
+      <c r="D71" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" t="s">
+        <v>191</v>
+      </c>
+      <c r="D72" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>226</v>
+      </c>
+      <c r="C73" t="s">
+        <v>191</v>
+      </c>
+      <c r="D73" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" t="s">
+        <v>226</v>
+      </c>
+      <c r="C74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" t="s">
+        <v>226</v>
+      </c>
+      <c r="C75" t="s">
+        <v>191</v>
+      </c>
+      <c r="D75" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" t="s">
+        <v>226</v>
+      </c>
+      <c r="C76" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" s="3">
+        <v>8.8888989089189201E+35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" t="s">
+        <v>226</v>
+      </c>
+      <c r="C79" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>118</v>
+      </c>
+      <c r="B80" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" t="s">
+        <v>225</v>
+      </c>
+      <c r="D81" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" t="s">
+        <v>225</v>
+      </c>
+      <c r="D82" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" t="s">
+        <v>226</v>
+      </c>
+      <c r="C84" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" t="s">
+        <v>226</v>
+      </c>
+      <c r="C85" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" t="s">
+        <v>225</v>
+      </c>
+      <c r="D86" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" t="s">
+        <v>226</v>
+      </c>
+      <c r="C87" t="s">
+        <v>225</v>
+      </c>
+      <c r="D87" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" t="s">
+        <v>225</v>
+      </c>
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" t="s">
+        <v>226</v>
+      </c>
+      <c r="C89" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" t="s">
+        <v>226</v>
+      </c>
+      <c r="C90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>226</v>
+      </c>
+      <c r="C91" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" t="s">
+        <v>226</v>
+      </c>
+      <c r="C92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>118</v>
+      </c>
+      <c r="B93" t="s">
+        <v>226</v>
+      </c>
+      <c r="C93" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" t="s">
+        <v>226</v>
+      </c>
+      <c r="C98" t="s">
+        <v>225</v>
+      </c>
+      <c r="D98" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" t="s">
+        <v>226</v>
+      </c>
+      <c r="C99" t="s">
+        <v>225</v>
+      </c>
+      <c r="D99" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" t="s">
+        <v>226</v>
+      </c>
+      <c r="C100" t="s">
+        <v>225</v>
+      </c>
+      <c r="D100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" t="s">
+        <v>226</v>
+      </c>
+      <c r="C101" t="s">
+        <v>225</v>
+      </c>
+      <c r="D101" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" t="s">
+        <v>226</v>
+      </c>
+      <c r="C102" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103" t="s">
+        <v>226</v>
+      </c>
+      <c r="C103" t="s">
+        <v>225</v>
+      </c>
+      <c r="D103" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" t="s">
+        <v>226</v>
+      </c>
+      <c r="C104" t="s">
+        <v>225</v>
+      </c>
+      <c r="D104" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" t="s">
+        <v>226</v>
+      </c>
+      <c r="C106" t="s">
+        <v>124</v>
+      </c>
+      <c r="D106" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" t="s">
+        <v>226</v>
+      </c>
+      <c r="C107" t="s">
+        <v>124</v>
+      </c>
+      <c r="D107" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108" t="s">
+        <v>124</v>
+      </c>
+      <c r="D108" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" t="s">
+        <v>226</v>
+      </c>
+      <c r="C109" t="s">
+        <v>124</v>
+      </c>
+      <c r="D109" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" t="s">
+        <v>226</v>
+      </c>
+      <c r="C110" t="s">
+        <v>124</v>
+      </c>
+      <c r="D110" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" t="s">
+        <v>124</v>
+      </c>
+      <c r="D111" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" t="s">
+        <v>226</v>
+      </c>
+      <c r="C112" t="s">
+        <v>124</v>
+      </c>
+      <c r="D112" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" t="s">
+        <v>124</v>
+      </c>
+      <c r="D113" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>118</v>
+      </c>
+      <c r="B114" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114" t="s">
+        <v>124</v>
+      </c>
+      <c r="D114" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" t="s">
+        <v>226</v>
+      </c>
+      <c r="C115" t="s">
+        <v>125</v>
+      </c>
+      <c r="D115" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" t="s">
+        <v>226</v>
+      </c>
+      <c r="C116" t="s">
+        <v>125</v>
+      </c>
+      <c r="D116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117" t="s">
+        <v>226</v>
+      </c>
+      <c r="C117" t="s">
+        <v>152</v>
+      </c>
+      <c r="D117" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>226</v>
+      </c>
+      <c r="C118" t="s">
+        <v>241</v>
+      </c>
+      <c r="D118" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>226</v>
+      </c>
+      <c r="C119" t="s">
+        <v>242</v>
+      </c>
+      <c r="D119" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>226</v>
+      </c>
+      <c r="C120" t="s">
+        <v>244</v>
+      </c>
+      <c r="D120" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>118</v>
+      </c>
+      <c r="B121" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" t="s">
+        <v>243</v>
+      </c>
+      <c r="D121" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>118</v>
+      </c>
+      <c r="B122" t="s">
+        <v>226</v>
+      </c>
+      <c r="C122" t="s">
+        <v>248</v>
+      </c>
+      <c r="D122">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="B123" t="s">
+        <v>249</v>
+      </c>
+      <c r="C123" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
scaling selected organism and population stats panes works now
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="2480" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="2480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="interface" sheetId="1" r:id="rId1"/>
@@ -1286,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
@@ -2582,7 +2582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hard coded setting default values on 'new' button
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="interface" sheetId="1" r:id="rId1"/>
     <sheet name="freezer" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="258">
   <si>
     <t>Page or Event</t>
   </si>
@@ -776,6 +777,24 @@
   </si>
   <si>
     <t>@ancestor</t>
+  </si>
+  <si>
+    <t>selected</t>
+  </si>
+  <si>
+    <t>popstats</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>popright</t>
+  </si>
+  <si>
+    <t>filler</t>
+  </si>
+  <si>
+    <t>=popright-filler(153/315</t>
   </si>
 </sst>
 </file>
@@ -829,7 +848,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -889,14 +908,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -926,6 +950,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,6 +981,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4277,4 +4305,76 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2">
+        <f>A2/A3</f>
+        <v>0.51428571428571423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <f>A1+A2</f>
+        <v>315</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>366</v>
+      </c>
+      <c r="B4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <f>A4-A3</f>
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
addes simple writing of json string to start a run
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="2480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="29080" yWindow="1760" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="interface" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="272">
   <si>
     <t>Page or Event</t>
   </si>
@@ -245,9 +245,6 @@
     <t>ancestral organsims</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t>boolean array of all cells w/ blue outlines based on which cells do what functions and are selcted. Goes to grid object rather than json directly, I think</t>
   </si>
   <si>
@@ -795,6 +792,51 @@
   </si>
   <si>
     <t>=popright-filler(153/315</t>
+  </si>
+  <si>
+    <t>boolean array</t>
+  </si>
+  <si>
+    <t>sizex</t>
+  </si>
+  <si>
+    <t>sizey</t>
+  </si>
+  <si>
+    <t>muteInput</t>
+  </si>
+  <si>
+    <t>notose</t>
+  </si>
+  <si>
+    <t>nanose</t>
+  </si>
+  <si>
+    <t>andose</t>
+  </si>
+  <si>
+    <t>ornose</t>
+  </si>
+  <si>
+    <t>orose</t>
+  </si>
+  <si>
+    <t>andnose</t>
+  </si>
+  <si>
+    <t>norose</t>
+  </si>
+  <si>
+    <t>xorose</t>
+  </si>
+  <si>
+    <t>equose</t>
+  </si>
+  <si>
+    <t>birthMethod</t>
+  </si>
+  <si>
+    <t>repeatMode</t>
   </si>
 </sst>
 </file>
@@ -848,8 +890,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -920,7 +964,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -952,6 +996,7 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -983,6 +1028,7 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1315,12 +1361,13 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1332,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1345,6 +1392,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>258</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -1356,6 +1406,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -1367,6 +1420,9 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -1378,6 +1434,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" t="s">
+        <v>270</v>
+      </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1448,9 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
@@ -1401,7 +1462,9 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1476,9 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
@@ -1425,7 +1490,9 @@
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -1437,7 +1504,9 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="D10" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1518,9 @@
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
@@ -1461,7 +1532,9 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
@@ -1473,7 +1546,9 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1560,9 @@
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
@@ -1497,7 +1574,9 @@
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -1777,7 +1856,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>257</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" t="s">
@@ -1792,7 +1871,7 @@
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" t="s">
@@ -1807,7 +1886,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" t="s">
@@ -1822,7 +1901,7 @@
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" t="s">
@@ -1837,7 +1916,7 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" t="s">
@@ -1852,7 +1931,7 @@
         <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" t="s">
@@ -1867,7 +1946,7 @@
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" t="s">
@@ -1882,7 +1961,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" t="s">
@@ -1897,7 +1976,7 @@
         <v>24</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
@@ -1916,7 +1995,7 @@
       </c>
       <c r="C48" s="1"/>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2113,7 +2192,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>19</v>
@@ -2125,26 +2204,26 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2153,53 +2232,53 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2208,391 +2287,391 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E83" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E84" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
         <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
         <v>37</v>
       </c>
       <c r="D87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E88" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" t="s">
         <v>4</v>
       </c>
       <c r="D89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B95" t="s">
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98" t="s">
+        <v>107</v>
+      </c>
+      <c r="D98" t="s">
         <v>108</v>
       </c>
-      <c r="D98" t="s">
-        <v>109</v>
-      </c>
       <c r="E98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E99" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D100" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E100" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D101" t="s">
+        <v>112</v>
+      </c>
+      <c r="E101" t="s">
         <v>113</v>
-      </c>
-      <c r="E101" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B102" t="s">
         <v>37</v>
       </c>
       <c r="D102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2611,7 +2690,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2624,1038 +2703,1038 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" t="s">
-        <v>122</v>
-      </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" t="s">
         <v>152</v>
-      </c>
-      <c r="D23" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
         <v>127</v>
-      </c>
-      <c r="C62" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" t="s">
         <v>186</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>187</v>
-      </c>
-      <c r="D64" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" t="s">
         <v>189</v>
-      </c>
-      <c r="C66" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C68" t="s">
+        <v>190</v>
+      </c>
+      <c r="D68" t="s">
         <v>191</v>
-      </c>
-      <c r="D68" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D77" s="3">
         <v>8.8888989089189201E+35</v>
@@ -3663,626 +3742,626 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D78" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C79" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B81" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C81" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B84" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D84" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B86" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C86" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D86" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D87" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D88" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D89" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C91" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D91" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B92" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B93" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D94" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B96" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C96" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C97" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C98" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D98" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C100" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D100" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B101" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D101" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C102" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B103" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C103" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D103" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B104" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
+        <v>225</v>
+      </c>
+      <c r="C105" t="s">
+        <v>125</v>
+      </c>
+      <c r="D105" t="s">
         <v>226</v>
-      </c>
-      <c r="C105" t="s">
-        <v>126</v>
-      </c>
-      <c r="D105" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B106" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C106" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D106" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B107" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C107" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C109" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B110" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C111" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D111" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C112" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B113" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C114" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D114" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C115" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D115" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D116" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C117" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D117" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C118" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C120" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B121" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C122" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D122">
         <v>1014</v>
@@ -4290,10 +4369,10 @@
     </row>
     <row r="123" spans="1:4">
       <c r="B123" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" t="s">
         <v>249</v>
-      </c>
-      <c r="C123" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4322,7 +4401,7 @@
         <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4330,7 +4409,7 @@
         <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2">
         <f>A2/A3</f>
@@ -4343,7 +4422,7 @@
         <v>315</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4351,7 +4430,7 @@
         <v>366</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4360,12 +4439,12 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 'need new Ancestor' dialog
</commit_message>
<xml_diff>
--- a/notes/dataInterface.xlsx
+++ b/notes/dataInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29080" yWindow="1760" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="interface" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="278">
   <si>
     <t>Page or Event</t>
   </si>
@@ -837,6 +837,24 @@
   </si>
   <si>
     <t>repeatMode</t>
+  </si>
+  <si>
+    <t>ancestor</t>
+  </si>
+  <si>
+    <t>list of string</t>
+  </si>
+  <si>
+    <t>gridAddress</t>
+  </si>
+  <si>
+    <t>list of xy pairs</t>
+  </si>
+  <si>
+    <t>location of each starting organism</t>
+  </si>
+  <si>
+    <t>starting organisms</t>
   </si>
 </sst>
 </file>
@@ -1358,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1432,41 +1450,41 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>261</v>
+      <c r="B6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" t="s">
+        <v>274</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>262</v>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1477,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1491,10 +1509,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1505,10 +1523,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1519,10 +1537,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1533,10 +1551,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1547,10 +1565,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1561,10 +1579,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1572,13 +1590,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1586,11 +1604,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1598,11 +1618,13 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1610,38 +1632,35 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1649,11 +1668,14 @@
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1661,14 +1683,11 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1676,11 +1695,11 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1688,11 +1707,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1700,11 +1722,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1716,7 +1738,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1728,7 +1750,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1740,7 +1762,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1752,7 +1774,7 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1764,7 +1786,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1776,7 +1798,7 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1788,7 +1810,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1800,7 +1822,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1812,7 +1834,7 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1824,7 +1846,7 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1836,7 +1858,7 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1848,7 +1870,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1856,14 +1878,11 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>257</v>
+        <v>19</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1871,14 +1890,11 @@
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>257</v>
+        <v>19</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1890,7 +1906,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
         <v>72</v>
@@ -1905,7 +1921,7 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
         <v>72</v>
@@ -1920,7 +1936,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E43" t="s">
         <v>72</v>
@@ -1935,7 +1951,7 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E44" t="s">
         <v>72</v>
@@ -1950,7 +1966,7 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E45" t="s">
         <v>72</v>
@@ -1965,7 +1981,7 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E46" t="s">
         <v>72</v>
@@ -1980,7 +1996,7 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E47" t="s">
         <v>72</v>
@@ -1991,62 +2007,68 @@
         <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>257</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>61</v>
+      </c>
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>37</v>
+        <v>257</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>62</v>
+      </c>
+      <c r="E49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -2055,10 +2077,10 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -2067,22 +2089,22 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -2091,22 +2113,22 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>24</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -2115,10 +2137,10 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -2127,10 +2149,10 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -2139,10 +2161,10 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -2151,10 +2173,10 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -2163,10 +2185,10 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -2175,10 +2197,10 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -2187,31 +2209,31 @@
       </c>
       <c r="C64" s="1"/>
       <c r="D64" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2219,54 +2241,54 @@
         <v>75</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="B69" s="1"/>
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C69" s="1"/>
+      <c r="D69" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>79</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C72" s="2"/>
+      <c r="B72" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="1"/>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>111</v>
+      </c>
+      <c r="E72" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2274,46 +2296,40 @@
         <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="B74" s="2"/>
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C74" s="2"/>
+      <c r="D74" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" t="s">
-        <v>92</v>
-      </c>
-      <c r="E75" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" t="s">
-        <v>78</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C76" s="1"/>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" t="s">
-        <v>113</v>
-      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
@@ -2324,7 +2340,7 @@
       </c>
       <c r="C77" s="1"/>
       <c r="D77" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E77" t="s">
         <v>113</v>
@@ -2339,7 +2355,7 @@
       </c>
       <c r="C78" s="1"/>
       <c r="D78" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E78" t="s">
         <v>113</v>
@@ -2354,7 +2370,7 @@
       </c>
       <c r="C79" s="1"/>
       <c r="D79" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E79" t="s">
         <v>113</v>
@@ -2369,7 +2385,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E80" t="s">
         <v>113</v>
@@ -2384,7 +2400,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E81" t="s">
         <v>113</v>
@@ -2399,7 +2415,7 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E82" t="s">
         <v>113</v>
@@ -2414,7 +2430,7 @@
       </c>
       <c r="C83" s="1"/>
       <c r="D83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E83" t="s">
         <v>113</v>
@@ -2429,7 +2445,7 @@
       </c>
       <c r="C84" s="1"/>
       <c r="D84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E84" t="s">
         <v>113</v>
@@ -2444,7 +2460,7 @@
       </c>
       <c r="C85" s="1"/>
       <c r="D85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E85" t="s">
         <v>113</v>
@@ -2454,11 +2470,12 @@
       <c r="A86" t="s">
         <v>78</v>
       </c>
-      <c r="B86" t="s">
-        <v>37</v>
-      </c>
+      <c r="B86" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="1"/>
       <c r="D86" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E86" t="s">
         <v>113</v>
@@ -2468,11 +2485,12 @@
       <c r="A87" t="s">
         <v>78</v>
       </c>
-      <c r="B87" t="s">
-        <v>37</v>
-      </c>
+      <c r="B87" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" s="1"/>
       <c r="D87" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E87" t="s">
         <v>113</v>
@@ -2483,10 +2501,10 @@
         <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E88" t="s">
         <v>113</v>
@@ -2497,10 +2515,10 @@
         <v>78</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D89" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E89" t="s">
         <v>113</v>
@@ -2514,7 +2532,7 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E90" t="s">
         <v>113</v>
@@ -2528,7 +2546,7 @@
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E91" t="s">
         <v>113</v>
@@ -2542,7 +2560,7 @@
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E92" t="s">
         <v>113</v>
@@ -2556,7 +2574,7 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E93" t="s">
         <v>113</v>
@@ -2570,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E94" t="s">
         <v>113</v>
@@ -2584,7 +2602,7 @@
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E95" t="s">
         <v>113</v>
@@ -2598,37 +2616,37 @@
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E96" t="s">
         <v>113</v>
       </c>
     </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>78</v>
+      </c>
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E98" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" t="s">
-        <v>105</v>
-      </c>
-      <c r="B99" t="s">
-        <v>107</v>
-      </c>
-      <c r="D99" t="s">
-        <v>109</v>
-      </c>
-      <c r="E99" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2640,7 +2658,7 @@
         <v>107</v>
       </c>
       <c r="D100" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E100" t="s">
         <v>113</v>
@@ -2654,7 +2672,7 @@
         <v>107</v>
       </c>
       <c r="D101" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E101" t="s">
         <v>113</v>
@@ -2665,12 +2683,40 @@
         <v>105</v>
       </c>
       <c r="B102" t="s">
+        <v>107</v>
+      </c>
+      <c r="D102" t="s">
+        <v>110</v>
+      </c>
+      <c r="E102" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>107</v>
+      </c>
+      <c r="D103" t="s">
+        <v>112</v>
+      </c>
+      <c r="E103" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" t="s">
         <v>37</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D104" t="s">
         <v>111</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E104" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>